<commit_message>
more data 231 responses + previous backup
</commit_message>
<xml_diff>
--- a/data/data.xlsx
+++ b/data/data.xlsx
@@ -10,8 +10,33 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment authorId="0" ref="G199">
+      <text>
+        <t xml:space="preserve">Responder updated this value.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="E225">
+      <text>
+        <t xml:space="preserve">Responder updated this value.</t>
+      </text>
+    </comment>
+    <comment authorId="0" ref="F225">
+      <text>
+        <t xml:space="preserve">Responder updated this value.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="885" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1361" uniqueCount="209">
   <si>
     <t>Timestamp</t>
   </si>
@@ -496,6 +521,265 @@
   <si>
     <t>Mobile banking
 Shopping online</t>
+  </si>
+  <si>
+    <t>Online Banking
+Ebay
+Jumia</t>
+  </si>
+  <si>
+    <t>Facebook ,whatsup mobile banking</t>
+  </si>
+  <si>
+    <t>Netflix,mcoopcash,equity,yoga,whatsapp</t>
+  </si>
+  <si>
+    <t>Safaricom
+PesaPap
+CBA Loop
+Jumia
+Alibaba</t>
+  </si>
+  <si>
+    <t>Facebook, WhatsApp,wish,jumia,kilimall,kcb
+Mozzilla,Operamini</t>
+  </si>
+  <si>
+    <t>Mshwari, safaricom app, mpesa, mcoop cash, opesa, okash</t>
+  </si>
+  <si>
+    <t>WhatsApp
+Facebook
+YouTube
+Telegram
+Twitter</t>
+  </si>
+  <si>
+    <t>Sim tool kit, premise, Facebook, WhatsApp and chrome</t>
+  </si>
+  <si>
+    <t>WhatsApp, Facebook</t>
+  </si>
+  <si>
+    <t>Uber. Jumia.</t>
+  </si>
+  <si>
+    <t>Facebook, WhatsApp, opera mini ,Mobile banking</t>
+  </si>
+  <si>
+    <t>Banking, mobile money</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safaricom app Jumia app </t>
+  </si>
+  <si>
+    <t>Whatsapp. E mail apps</t>
+  </si>
+  <si>
+    <t>+254702277923</t>
+  </si>
+  <si>
+    <t>Jumia,Kilimall,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Banking apps 
+Facebook 
+WhatsApp 
+Microsoft outlook 
+Gmail 
+Twitter 
+Jumia shopping app
+Mysafaricom
+</t>
+  </si>
+  <si>
+    <t>goodle app-30%
+playstore -30%
+equity-20%
+facebook-70%
+whattup-60%</t>
+  </si>
+  <si>
+    <t>Mobile banking, GPS, microsoft office</t>
+  </si>
+  <si>
+    <t>Facebook, Xclub, Brave</t>
+  </si>
+  <si>
+    <t>Facebook
+Whatsap
+Whatsap business
+Instagram 
+Twitter
+Jiji</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Safaricom app
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equity, Jumia, </t>
+  </si>
+  <si>
+    <t>Eazzy banking app</t>
+  </si>
+  <si>
+    <t>I don't use any</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Whatsapp, Facebook, futmob, Google, chrome ,dictionary ,safaricom </t>
+  </si>
+  <si>
+    <t>Timiza
+Branch
+Tala
+Amazon
+Jumia</t>
+  </si>
+  <si>
+    <t>I do not use any</t>
+  </si>
+  <si>
+    <t>Jumia, kilimall, co-op cash</t>
+  </si>
+  <si>
+    <t>Jumia,kilimall</t>
+  </si>
+  <si>
+    <t>Jumia, Killmall</t>
+  </si>
+  <si>
+    <t>Whatsapp,facebook</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Barclays
+Alibaba
+Jumia
+KCB
+</t>
+  </si>
+  <si>
+    <t>National Bank of Kenya, KCB, BARCLAYS</t>
+  </si>
+  <si>
+    <t>Mcoop app, Jumia force, Tala</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Equity Banks, Jumia, Fuzu, Brighter Monday, KCB app, Killimall app, alfalafa, Pesapal, Airtel, Safaricom, </t>
+  </si>
+  <si>
+    <t>Jumia shopping mall
+Tala loan app
+Branch loan app
+Gotv app
+Sidian bank app</t>
+  </si>
+  <si>
+    <t>ALIBABA, KCB, JUMIA, PAYPAL</t>
+  </si>
+  <si>
+    <t>Safaricom App
+CBA Loop
+Airtel App
+Equity Bank
+Jumia App</t>
+  </si>
+  <si>
+    <t>Equity, PayPal</t>
+  </si>
+  <si>
+    <t>Watsapp,facebook,instagram</t>
+  </si>
+  <si>
+    <t>Safaricom App,  Airtel App,  Eazzy Banking,  Branch App</t>
+  </si>
+  <si>
+    <t>Watsup</t>
+  </si>
+  <si>
+    <t>Kcb kra itax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kcb bank app
+Mpesa mobile app
+Kilimall 
+Jumia
+Nairobi county council epayment app
+Kenya power </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facebook, Twitter, kcb, Gmail, LinkedIn </t>
+  </si>
+  <si>
+    <t>Jumia app, Equity app</t>
+  </si>
+  <si>
+    <t>Jumia
+Kilimall
+Geopoll</t>
+  </si>
+  <si>
+    <t>Jiji</t>
+  </si>
+  <si>
+    <t>Kcb bank,  Tala loans,  PayPal app</t>
+  </si>
+  <si>
+    <t>Mula,kcb,uber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On line marketing mobile money transfer, beting </t>
+  </si>
+  <si>
+    <t>Tala, co-op  mobile banking,  kcb</t>
+  </si>
+  <si>
+    <t>Jumia and kilimall</t>
+  </si>
+  <si>
+    <t>Eco bank,KCB,paypal</t>
+  </si>
+  <si>
+    <t>Tala
+Pesapap
+Eazzy Banking
+Branch
+Jumia
+Alibaba
+Kilimall</t>
+  </si>
+  <si>
+    <t>Whatsapp,facebook,jumia,alibaba</t>
+  </si>
+  <si>
+    <t>Jumia,Tala,Killimall</t>
+  </si>
+  <si>
+    <t>KCB bank app, equity mobile banking app,tala app, PayPal,Bitcoin ,cash app</t>
+  </si>
+  <si>
+    <t>Equity azzypay, tala, timiza,branch, jumia,kilimall</t>
+  </si>
+  <si>
+    <t>Eazzy banking
+Jumia
+Aliexpress</t>
+  </si>
+  <si>
+    <t>Jumia
+Tingg
+Kilimall
+Eazypay
+Mygotv</t>
+  </si>
+  <si>
+    <t>Lipa na mpesa</t>
+  </si>
+  <si>
+    <t>Kcb app</t>
   </si>
 </sst>
 </file>
@@ -4890,7 +5174,7 @@
       </c>
     </row>
     <row r="120">
-      <c r="A120" s="5">
+      <c r="A120" s="3">
         <v>43756.55600193287</v>
       </c>
       <c r="B120" s="4" t="s">
@@ -5997,7 +6281,2822 @@
         <v>16</v>
       </c>
     </row>
+    <row r="152">
+      <c r="A152" s="3">
+        <v>43775.33296368056</v>
+      </c>
+      <c r="B152" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C152" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D152" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E152" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="F152" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G152" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="H152" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I152" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J152" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K152" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" s="3">
+        <v>43781.227902557875</v>
+      </c>
+      <c r="B153" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C153" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D153" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E153" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F153" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G153" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="H153" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I153" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J153" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="K153" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" s="3">
+        <v>43781.23763131944</v>
+      </c>
+      <c r="B154" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C154" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D154" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E154" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F154" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G154" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="H154" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I154" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J154" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="K154" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" s="3">
+        <v>43781.24102001157</v>
+      </c>
+      <c r="B155" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C155" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D155" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E155" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="F155" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="G155" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H155" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I155" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J155" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="K155" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" s="3">
+        <v>43781.258837534726</v>
+      </c>
+      <c r="B156" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C156" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D156" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E156" s="4">
+        <v>40.0</v>
+      </c>
+      <c r="F156" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="H156" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I156" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J156" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="K156" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" s="3">
+        <v>43781.30567173611</v>
+      </c>
+      <c r="B157" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C157" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D157" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E157" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F157" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="H157" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I157" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J157" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K157" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" s="3">
+        <v>43781.32149771991</v>
+      </c>
+      <c r="B158" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C158" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D158" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E158" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="F158" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="G158" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="H158" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I158" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J158" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K158" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" s="3">
+        <v>43781.33762064815</v>
+      </c>
+      <c r="B159" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C159" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D159" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E159" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F159" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G159" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="H159" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I159" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J159" s="4">
+        <v>29.0</v>
+      </c>
+      <c r="K159" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="3">
+        <v>43781.35790513889</v>
+      </c>
+      <c r="B160" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C160" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D160" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E160" s="4">
+        <v>15.0</v>
+      </c>
+      <c r="F160" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G160" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H160" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I160" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J160" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K160" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" s="3">
+        <v>43781.389110937496</v>
+      </c>
+      <c r="B161" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C161" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D161" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E161" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="F161" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G161" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H161" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I161" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J161" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="K161" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" s="3">
+        <v>43781.42821704861</v>
+      </c>
+      <c r="B162" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C162" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D162" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E162" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F162" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G162" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="H162" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I162" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J162" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K162" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" s="3">
+        <v>43781.48045819445</v>
+      </c>
+      <c r="B163" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C163" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D163" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E163" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F163" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G163" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="H163" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I163" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J163" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="K163" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" s="3">
+        <v>43781.50480040509</v>
+      </c>
+      <c r="B164" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C164" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D164" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E164" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F164" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G164" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H164" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I164" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J164" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K164" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" s="3">
+        <v>43781.51103356481</v>
+      </c>
+      <c r="B165" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C165" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D165" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E165" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F165" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G165" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="H165" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I165" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J165" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="K165" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" s="3">
+        <v>43781.523167974534</v>
+      </c>
+      <c r="B166" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C166" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D166" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E166" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F166" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G166" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="H166" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I166" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J166" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="K166" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" s="3">
+        <v>43781.55850833333</v>
+      </c>
+      <c r="B167" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C167" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D167" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E167" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="F167" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H167" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I167" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J167" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="K167" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" s="3">
+        <v>43781.56468563658</v>
+      </c>
+      <c r="B168" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C168" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D168" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E168" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F168" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G168" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="H168" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I168" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J168" s="4">
+        <v>90.0</v>
+      </c>
+      <c r="K168" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" s="3">
+        <v>43781.57141063658</v>
+      </c>
+      <c r="B169" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C169" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D169" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E169" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F169" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G169" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="H169" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I169" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J169" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="K169" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" s="3">
+        <v>43781.589936550925</v>
+      </c>
+      <c r="B170" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C170" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="D170" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E170" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="F170" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G170" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="H170" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I170" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J170" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="K170" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" s="3">
+        <v>43781.59064148148</v>
+      </c>
+      <c r="B171" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C171" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D171" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E171" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="F171" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="G171" s="4" t="s">
+        <v>160</v>
+      </c>
+      <c r="H171" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I171" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J171" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K171" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" s="3">
+        <v>43781.596218645835</v>
+      </c>
+      <c r="B172" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C172" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D172" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E172" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F172" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G172" s="4" t="s">
+        <v>161</v>
+      </c>
+      <c r="H172" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I172" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J172" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K172" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" s="3">
+        <v>43781.66339623842</v>
+      </c>
+      <c r="B173" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C173" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D173" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E173" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="F173" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="H173" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I173" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J173" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="K173" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" s="3">
+        <v>43781.674087708336</v>
+      </c>
+      <c r="B174" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C174" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D174" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E174" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F174" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G174" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="H174" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I174" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J174" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K174" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" s="3">
+        <v>43781.689613009265</v>
+      </c>
+      <c r="B175" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C175" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D175" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E175" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="F175" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="G175" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="H175" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I175" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J175" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="K175" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" s="3">
+        <v>43781.716263009264</v>
+      </c>
+      <c r="B176" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C176" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D176" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E176" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F176" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G176" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="H176" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I176" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J176" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K176" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" s="3">
+        <v>43781.74625833333</v>
+      </c>
+      <c r="B177" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C177" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D177" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E177" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F177" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="H177" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I177" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J177" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K177" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" s="3">
+        <v>43781.753914375004</v>
+      </c>
+      <c r="B178" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C178" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D178" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E178" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="F178" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G178" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="H178" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I178" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J178" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="K178" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" s="3">
+        <v>43781.76625729167</v>
+      </c>
+      <c r="B179" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C179" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D179" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E179" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F179" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G179" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="H179" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I179" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J179" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K179" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" s="3">
+        <v>43781.801237604166</v>
+      </c>
+      <c r="B180" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C180" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D180" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E180" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="F180" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G180" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H180" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I180" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J180" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="K180" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" s="3">
+        <v>43781.83349634259</v>
+      </c>
+      <c r="B181" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C181" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D181" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E181" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="F181" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G181" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="H181" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I181" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J181" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="K181" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" s="3">
+        <v>43781.86270550926</v>
+      </c>
+      <c r="B182" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C182" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D182" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E182" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F182" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G182" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="H182" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I182" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J182" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="K182" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" s="3">
+        <v>43781.911414120375</v>
+      </c>
+      <c r="B183" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C183" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D183" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E183" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F183" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G183" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="H183" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I183" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J183" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="K183" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" s="3">
+        <v>43781.92712395833</v>
+      </c>
+      <c r="B184" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C184" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D184" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E184" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F184" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G184" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="H184" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I184" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J184" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K184" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" s="3">
+        <v>43781.93729341435</v>
+      </c>
+      <c r="B185" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C185" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D185" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E185" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="F185" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G185" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="H185" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I185" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J185" s="4">
+        <v>12.0</v>
+      </c>
+      <c r="K185" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" s="3">
+        <v>43782.41464099537</v>
+      </c>
+      <c r="B186" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C186" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D186" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E186" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="F186" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G186" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="H186" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I186" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J186" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="K186" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" s="3">
+        <v>43782.442589328704</v>
+      </c>
+      <c r="B187" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C187" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D187" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E187" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F187" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G187" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="H187" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I187" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J187" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K187" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" s="3">
+        <v>43782.4450894676</v>
+      </c>
+      <c r="B188" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C188" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D188" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E188" s="4">
+        <v>12.0</v>
+      </c>
+      <c r="F188" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G188" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="H188" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I188" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J188" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="K188" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" s="3">
+        <v>43782.470383935186</v>
+      </c>
+      <c r="B189" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C189" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D189" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E189" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F189" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G189" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="H189" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I189" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J189" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K189" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" s="3">
+        <v>43782.56146324074</v>
+      </c>
+      <c r="B190" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C190" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D190" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E190" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="F190" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G190" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="H190" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I190" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J190" s="4">
+        <v>15.0</v>
+      </c>
+      <c r="K190" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" s="3">
+        <v>43782.707511932866</v>
+      </c>
+      <c r="B191" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C191" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D191" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E191" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="F191" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G191" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="H191" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I191" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J191" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K191" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" s="3">
+        <v>43782.79547403935</v>
+      </c>
+      <c r="B192" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C192" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D192" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E192" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F192" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G192" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="H192" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I192" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J192" s="4">
+        <v>18.0</v>
+      </c>
+      <c r="K192" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" s="3">
+        <v>43782.81614282407</v>
+      </c>
+      <c r="B193" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C193" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D193" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E193" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="F193" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G193" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="H193" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I193" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J193" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K193" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" s="3">
+        <v>43782.86356616898</v>
+      </c>
+      <c r="B194" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C194" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D194" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E194" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="F194" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G194" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="H194" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I194" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J194" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="K194" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" s="3">
+        <v>43782.89999032408</v>
+      </c>
+      <c r="B195" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C195" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D195" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E195" s="4">
+        <v>15.0</v>
+      </c>
+      <c r="F195" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="G195" s="4" t="s">
+        <v>180</v>
+      </c>
+      <c r="H195" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I195" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J195" s="4">
+        <v>15.0</v>
+      </c>
+      <c r="K195" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" s="3">
+        <v>43782.91338297454</v>
+      </c>
+      <c r="B196" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C196" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D196" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E196" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F196" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G196" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="H196" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I196" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J196" s="4">
+        <v>16.0</v>
+      </c>
+      <c r="K196" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" s="3">
+        <v>43782.94697710648</v>
+      </c>
+      <c r="B197" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C197" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D197" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E197" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F197" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G197" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H197" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I197" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J197" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="K197" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" s="3">
+        <v>43783.00131537037</v>
+      </c>
+      <c r="B198" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C198" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D198" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E198" s="4">
+        <v>40.0</v>
+      </c>
+      <c r="F198" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="G198" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="H198" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I198" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J198" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="K198" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" s="5">
+        <v>43783.17069846065</v>
+      </c>
+      <c r="B199" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C199" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D199" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E199" s="4">
+        <v>15.0</v>
+      </c>
+      <c r="F199" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G199" s="4" t="s">
+        <v>183</v>
+      </c>
+      <c r="H199" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I199" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J199" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K199" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="200">
+      <c r="A200" s="3">
+        <v>43783.32672173611</v>
+      </c>
+      <c r="B200" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C200" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D200" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E200" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="F200" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G200" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="H200" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I200" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J200" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="K200" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" s="3">
+        <v>43783.63794152778</v>
+      </c>
+      <c r="B201" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C201" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D201" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E201" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F201" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G201" s="4" t="s">
+        <v>185</v>
+      </c>
+      <c r="H201" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I201" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J201" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K201" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" s="3">
+        <v>43783.659539953704</v>
+      </c>
+      <c r="B202" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C202" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D202" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E202" s="4">
+        <v>15.0</v>
+      </c>
+      <c r="F202" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G202" s="4" t="s">
+        <v>186</v>
+      </c>
+      <c r="H202" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I202" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J202" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="K202" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" s="3">
+        <v>43783.70256497685</v>
+      </c>
+      <c r="B203" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C203" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D203" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E203" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F203" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G203" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="H203" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I203" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J203" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="K203" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" s="3">
+        <v>43784.06125423611</v>
+      </c>
+      <c r="B204" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C204" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D204" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E204" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F204" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G204" s="4" t="s">
+        <v>188</v>
+      </c>
+      <c r="H204" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I204" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J204" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K204" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" s="3">
+        <v>43784.143684317125</v>
+      </c>
+      <c r="B205" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C205" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D205" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E205" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="F205" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G205" s="4" t="s">
+        <v>189</v>
+      </c>
+      <c r="H205" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I205" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J205" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K205" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" s="3">
+        <v>43784.16419993056</v>
+      </c>
+      <c r="B206" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C206" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D206" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E206" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F206" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G206" s="4" t="s">
+        <v>190</v>
+      </c>
+      <c r="H206" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I206" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J206" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="K206" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" s="3">
+        <v>43784.19601127315</v>
+      </c>
+      <c r="B207" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C207" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D207" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E207" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F207" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G207" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="H207" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I207" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J207" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="K207" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" s="3">
+        <v>43784.44470600694</v>
+      </c>
+      <c r="B208" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C208" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D208" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E208" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="F208" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G208" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="H208" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I208" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J208" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="K208" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" s="3">
+        <v>43784.49412662037</v>
+      </c>
+      <c r="B209" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C209" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D209" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E209" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="F209" s="4">
+        <v>13.0</v>
+      </c>
+      <c r="H209" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I209" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J209" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="K209" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" s="3">
+        <v>43784.739842546296</v>
+      </c>
+      <c r="B210" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C210" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D210" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E210" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="F210" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="H210" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I210" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J210" s="4">
+        <v>24.0</v>
+      </c>
+      <c r="K210" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" s="3">
+        <v>43784.81563679398</v>
+      </c>
+      <c r="B211" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C211" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D211" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E211" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F211" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G211" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="H211" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I211" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J211" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K211" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" s="3">
+        <v>43784.83102844907</v>
+      </c>
+      <c r="B212" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C212" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D212" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E212" s="4">
+        <v>13.0</v>
+      </c>
+      <c r="F212" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G212" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="H212" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I212" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J212" s="4">
+        <v>24.0</v>
+      </c>
+      <c r="K212" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="213">
+      <c r="A213" s="3">
+        <v>43784.90258222222</v>
+      </c>
+      <c r="B213" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C213" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D213" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E213" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="F213" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G213" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="H213" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I213" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J213" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K213" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" s="3">
+        <v>43785.12011046296</v>
+      </c>
+      <c r="B214" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C214" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D214" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E214" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="F214" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G214" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="H214" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I214" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J214" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="K214" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" s="3">
+        <v>43785.15918831019</v>
+      </c>
+      <c r="B215" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C215" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D215" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E215" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F215" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G215" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="H215" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I215" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J215" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="K215" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" s="3">
+        <v>43785.18811053241</v>
+      </c>
+      <c r="B216" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C216" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="D216" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E216" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F216" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G216" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="H216" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I216" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J216" s="4">
+        <v>14.0</v>
+      </c>
+      <c r="K216" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" s="3">
+        <v>43785.20369552083</v>
+      </c>
+      <c r="B217" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C217" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D217" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E217" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F217" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G217" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="H217" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I217" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J217" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="K217" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" s="3">
+        <v>43785.21520157407</v>
+      </c>
+      <c r="B218" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C218" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D218" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E218" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="F218" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G218" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="H218" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I218" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J218" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K218" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" s="3">
+        <v>43785.586392847224</v>
+      </c>
+      <c r="B219" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C219" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D219" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E219" s="4">
+        <v>15.0</v>
+      </c>
+      <c r="F219" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="G219" s="4" t="s">
+        <v>200</v>
+      </c>
+      <c r="H219" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I219" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J219" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="K219" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" s="3">
+        <v>43785.598308368055</v>
+      </c>
+      <c r="B220" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C220" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D220" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E220" s="4">
+        <v>17.0</v>
+      </c>
+      <c r="F220" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G220" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H220" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I220" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J220" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K220" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" s="3">
+        <v>43785.683774641206</v>
+      </c>
+      <c r="B221" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C221" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D221" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E221" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F221" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G221" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="H221" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I221" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J221" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="K221" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" s="3">
+        <v>43785.75157288194</v>
+      </c>
+      <c r="B222" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C222" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D222" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E222" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F222" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="G222" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="H222" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I222" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J222" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K222" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="223">
+      <c r="A223" s="3">
+        <v>43785.805021736116</v>
+      </c>
+      <c r="B223" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C223" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D223" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E223" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F223" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G223" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="H223" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I223" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="J223" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="K223" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" s="3">
+        <v>43786.00752590278</v>
+      </c>
+      <c r="B224" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C224" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D224" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E224" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="F224" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G224" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="H224" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I224" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J224" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K224" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" s="5">
+        <v>43786.046129560185</v>
+      </c>
+      <c r="B225" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C225" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D225" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E225" s="4">
+        <v>20.0</v>
+      </c>
+      <c r="F225" s="4">
+        <v>8.0</v>
+      </c>
+      <c r="G225" s="4" t="s">
+        <v>204</v>
+      </c>
+      <c r="H225" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I225" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="J225" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="K225" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" s="3">
+        <v>43786.0555196875</v>
+      </c>
+      <c r="B226" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C226" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D226" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E226" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="F226" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G226" s="4" t="s">
+        <v>205</v>
+      </c>
+      <c r="H226" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="I226" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="J226" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="K226" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" s="3">
+        <v>43786.182956273144</v>
+      </c>
+      <c r="B227" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C227" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D227" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E227" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F227" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G227" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H227" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I227" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J227" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="K227" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="228">
+      <c r="A228" s="3">
+        <v>43786.18309506944</v>
+      </c>
+      <c r="B228" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C228" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D228" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E228" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F228" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G228" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="H228" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I228" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J228" s="4">
+        <v>7.0</v>
+      </c>
+      <c r="K228" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="229">
+      <c r="A229" s="3">
+        <v>43786.34372980324</v>
+      </c>
+      <c r="B229" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C229" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="D229" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E229" s="4">
+        <v>30.0</v>
+      </c>
+      <c r="F229" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="G229" s="4" t="s">
+        <v>206</v>
+      </c>
+      <c r="H229" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="I229" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J229" s="4">
+        <v>9.0</v>
+      </c>
+      <c r="K229" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" s="5">
+        <v>43786.38013276621</v>
+      </c>
+      <c r="B230" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C230" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="D230" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="E230" s="4">
+        <v>5.0</v>
+      </c>
+      <c r="F230" s="4">
+        <v>3.0</v>
+      </c>
+      <c r="G230" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="H230" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I230" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="J230" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="K230" s="4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="231">
+      <c r="A231" s="3">
+        <v>43786.43272239583</v>
+      </c>
+      <c r="B231" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C231" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D231" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E231" s="4">
+        <v>6.0</v>
+      </c>
+      <c r="F231" s="4">
+        <v>1.0</v>
+      </c>
+      <c r="G231" s="4" t="s">
+        <v>207</v>
+      </c>
+      <c r="H231" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I231" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J231" s="4">
+        <v>25.0</v>
+      </c>
+      <c r="K231" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" s="3">
+        <v>43786.53499021991</v>
+      </c>
+      <c r="B232" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C232" s="4">
+        <v>2.0</v>
+      </c>
+      <c r="D232" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E232" s="4">
+        <v>4.0</v>
+      </c>
+      <c r="F232" s="4">
+        <v>0.0</v>
+      </c>
+      <c r="G232" s="4" t="s">
+        <v>208</v>
+      </c>
+      <c r="H232" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I232" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="J232" s="4">
+        <v>10.0</v>
+      </c>
+      <c r="K232" s="4" t="s">
+        <v>24</v>
+      </c>
+    </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>